<commit_message>
update diagrams according to feedback
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi_\Dropbox\_zhaw\21FS\BA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Dropbox\_Schule\_zhaw\21FS\BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A49B2-7B94-410C-8BC7-2DEA461E076D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402A45DA-2633-46B4-B1DF-D10393DCEEF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
+    <workbookView xWindow="3440" yWindow="3030" windowWidth="20260" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,7 +472,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -770,30 +770,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BAD31A-C75F-4250-BB4F-3B614CCB7A8D}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.21875" style="1"/>
-    <col min="7" max="7" width="11.77734375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -816,7 +816,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>50</v>
       </c>
@@ -839,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>6</v>
       </c>
@@ -862,7 +862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="34">
         <v>8</v>
       </c>
@@ -879,7 +879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="36"/>
       <c r="B6" s="6">
         <v>44249</v>
@@ -894,7 +894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="35"/>
       <c r="B7" s="6">
         <v>44252</v>
@@ -909,7 +909,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="34">
         <v>9</v>
       </c>
@@ -926,7 +926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
       <c r="B9" s="6">
         <v>44256</v>
@@ -941,7 +941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
       <c r="B10" s="6">
         <v>44259</v>
@@ -956,7 +956,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="34">
         <v>10</v>
       </c>
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="36"/>
       <c r="B12" s="9" t="s">
         <v>1</v>
@@ -994,7 +994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
       <c r="B13" s="6">
         <v>44263</v>
@@ -1012,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="35"/>
       <c r="B14" s="6">
         <v>44266</v>
@@ -1030,7 +1030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="38">
         <v>11</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="38"/>
       <c r="B16" s="9" t="s">
         <v>1</v>
@@ -1062,7 +1062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="38"/>
       <c r="B17" s="6">
         <v>44270</v>
@@ -1077,7 +1077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="6">
         <v>44273</v>
@@ -1092,7 +1092,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="34">
         <v>12</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="36"/>
       <c r="B20" s="9" t="s">
         <v>1</v>
@@ -1124,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="36"/>
       <c r="B21" s="6">
         <v>44277</v>
@@ -1139,7 +1139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="35"/>
       <c r="B22" s="6">
         <v>44280</v>
@@ -1154,7 +1154,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="34">
         <v>13</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="36"/>
       <c r="B24" s="9" t="s">
         <v>1</v>
@@ -1186,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="36"/>
       <c r="B25" s="6">
         <v>44284</v>
@@ -1201,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="35"/>
       <c r="B26" s="6">
         <v>44287</v>
@@ -1216,7 +1216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="34">
         <v>14</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="36"/>
       <c r="B28" s="9" t="s">
         <v>1</v>
@@ -1248,7 +1248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="36"/>
       <c r="B29" s="6">
         <v>44291</v>
@@ -1263,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="35"/>
       <c r="B30" s="6">
         <v>44294</v>
@@ -1278,7 +1278,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="34">
         <v>15</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="36"/>
       <c r="B32" s="9" t="s">
         <v>1</v>
@@ -1310,7 +1310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="36"/>
       <c r="B33" s="6">
         <v>44298</v>
@@ -1325,7 +1325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="35"/>
       <c r="B34" s="6">
         <v>44301</v>
@@ -1340,7 +1340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="34">
         <v>16</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="36"/>
       <c r="B36" s="9" t="s">
         <v>1</v>
@@ -1372,7 +1372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="36"/>
       <c r="B37" s="6">
         <v>44305</v>
@@ -1387,7 +1387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="35"/>
       <c r="B38" s="6">
         <v>44308</v>
@@ -1402,7 +1402,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="34">
         <v>17</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="36"/>
       <c r="B40" s="9" t="s">
         <v>1</v>
@@ -1434,7 +1434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="36"/>
       <c r="B41" s="6">
         <v>44312</v>
@@ -1449,7 +1449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="35"/>
       <c r="B42" s="6">
         <v>44315</v>
@@ -1464,7 +1464,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="34">
         <v>18</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="36"/>
       <c r="B44" s="9" t="s">
         <v>1</v>
@@ -1496,7 +1496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="36"/>
       <c r="B45" s="6">
         <v>44319</v>
@@ -1511,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="35"/>
       <c r="B46" s="6">
         <v>44322</v>
@@ -1526,7 +1526,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="34">
         <v>19</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="36"/>
       <c r="B48" s="9" t="s">
         <v>1</v>
@@ -1558,7 +1558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="36"/>
       <c r="B49" s="6">
         <v>44326</v>
@@ -1573,7 +1573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="35"/>
       <c r="B50" s="6">
         <v>44329</v>
@@ -1588,7 +1588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="34">
         <v>20</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="36"/>
       <c r="B52" s="9" t="s">
         <v>1</v>
@@ -1620,7 +1620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="36"/>
       <c r="B53" s="25" t="s">
         <v>1</v>
@@ -1635,7 +1635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="36"/>
       <c r="B54" s="6">
         <v>44333</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="35"/>
       <c r="B55" s="6">
         <v>44336</v>
@@ -1665,7 +1665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="34">
         <v>21</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="36"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
@@ -1697,7 +1697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="36"/>
       <c r="B58" s="6">
         <v>44340</v>
@@ -1712,7 +1712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="35"/>
       <c r="B59" s="6">
         <v>44343</v>
@@ -1727,7 +1727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="34">
         <v>22</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="36"/>
       <c r="B61" s="3" t="s">
         <v>1</v>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="36"/>
       <c r="B62" s="6">
         <v>44347</v>
@@ -1772,7 +1772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="35"/>
       <c r="B63" s="6">
         <v>44350</v>
@@ -1787,7 +1787,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="34">
         <v>23</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="35"/>
       <c r="B65" s="14">
         <v>44358</v>
@@ -1817,7 +1817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="34" t="s">
         <v>17</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="35"/>
       <c r="B67" s="31">
         <v>44383</v>

</xml_diff>

<commit_message>
update timetable, update requirements
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Dropbox\_Schule\_zhaw\21FS\BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402A45DA-2633-46B4-B1DF-D10393DCEEF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46EB088-D7E1-4724-B873-685F4DA13E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="3030" windowWidth="20260" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
+    <workbookView xWindow="0" yWindow="3250" windowWidth="26570" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +222,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -332,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,20 +440,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BAD31A-C75F-4250-BB4F-3B614CCB7A8D}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,11 +803,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -863,7 +879,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
+      <c r="A5" s="36">
         <v>8</v>
       </c>
       <c r="B5" s="3">
@@ -880,7 +896,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="6">
         <v>44249</v>
       </c>
@@ -895,7 +911,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="35"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="6">
         <v>44252</v>
       </c>
@@ -910,7 +926,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="34">
+      <c r="A8" s="36">
         <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -927,7 +943,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="6">
         <v>44256</v>
       </c>
@@ -942,7 +958,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="6">
         <v>44259</v>
       </c>
@@ -957,7 +973,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="34">
+      <c r="A11" s="36">
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
@@ -977,7 +993,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="9" t="s">
         <v>1</v>
       </c>
@@ -995,7 +1011,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="6">
         <v>44263</v>
       </c>
@@ -1013,7 +1029,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="6">
         <v>44266</v>
       </c>
@@ -1031,7 +1047,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="38">
+      <c r="A15" s="35">
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -1048,7 +1064,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
@@ -1063,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="6">
         <v>44270</v>
       </c>
@@ -1078,7 +1094,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="6">
         <v>44273</v>
       </c>
@@ -1093,7 +1109,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="34">
+      <c r="A19" s="36">
         <v>12</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -1110,7 +1126,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="9" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1141,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="6">
         <v>44277</v>
       </c>
@@ -1140,7 +1156,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="6">
         <v>44280</v>
       </c>
@@ -1155,7 +1171,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="34">
+      <c r="A23" s="36">
         <v>13</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -1172,7 +1188,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="36"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="9" t="s">
         <v>1</v>
       </c>
@@ -1187,7 +1203,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="6">
         <v>44284</v>
       </c>
@@ -1202,7 +1218,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="35"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="6">
         <v>44287</v>
       </c>
@@ -1217,7 +1233,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="34">
+      <c r="A27" s="36">
         <v>14</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -1234,7 +1250,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="36"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
@@ -1249,7 +1265,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="36"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="6">
         <v>44291</v>
       </c>
@@ -1264,7 +1280,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="35"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="6">
         <v>44294</v>
       </c>
@@ -1279,7 +1295,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="34">
+      <c r="A31" s="36">
         <v>15</v>
       </c>
       <c r="B31" s="21" t="s">
@@ -1296,7 +1312,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="36"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="9" t="s">
         <v>1</v>
       </c>
@@ -1311,7 +1327,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="36"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="6">
         <v>44298</v>
       </c>
@@ -1326,7 +1342,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="35"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="6">
         <v>44301</v>
       </c>
@@ -1341,7 +1357,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="34">
+      <c r="A35" s="36">
         <v>16</v>
       </c>
       <c r="B35" s="21" t="s">
@@ -1358,7 +1374,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="36"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="9" t="s">
         <v>1</v>
       </c>
@@ -1373,7 +1389,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="36"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="6">
         <v>44305</v>
       </c>
@@ -1388,7 +1404,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="35"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="6">
         <v>44308</v>
       </c>
@@ -1403,7 +1419,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="34">
+      <c r="A39" s="36">
         <v>17</v>
       </c>
       <c r="B39" s="21" t="s">
@@ -1420,7 +1436,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="36"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
@@ -1435,22 +1451,22 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="36"/>
-      <c r="B41" s="6">
+      <c r="A41" s="37"/>
+      <c r="B41" s="39">
         <v>44312</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="8" t="s">
+      <c r="D41" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="35"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="6">
         <v>44315</v>
       </c>
@@ -1465,7 +1481,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="34">
+      <c r="A43" s="36">
         <v>18</v>
       </c>
       <c r="B43" s="21" t="s">
@@ -1482,7 +1498,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="36"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="9" t="s">
         <v>1</v>
       </c>
@@ -1497,7 +1513,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="36"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="6">
         <v>44319</v>
       </c>
@@ -1512,7 +1528,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="35"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="6">
         <v>44322</v>
       </c>
@@ -1527,7 +1543,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="34">
+      <c r="A47" s="36">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
@@ -1544,7 +1560,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="36"/>
+      <c r="A48" s="37"/>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
@@ -1559,7 +1575,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="36"/>
+      <c r="A49" s="37"/>
       <c r="B49" s="6">
         <v>44326</v>
       </c>
@@ -1574,22 +1590,22 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="35"/>
-      <c r="B50" s="6">
+      <c r="A50" s="38"/>
+      <c r="B50" s="39">
         <v>44329</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="8" t="s">
+      <c r="D50" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="41" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="34">
+      <c r="A51" s="36">
         <v>20</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -1606,7 +1622,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="36"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
@@ -1621,7 +1637,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
@@ -1636,7 +1652,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="6">
         <v>44333</v>
       </c>
@@ -1651,7 +1667,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="35"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="6">
         <v>44336</v>
       </c>
@@ -1666,7 +1682,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="34">
+      <c r="A56" s="36">
         <v>21</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -1683,7 +1699,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="36"/>
+      <c r="A57" s="37"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -1698,7 +1714,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="36"/>
+      <c r="A58" s="37"/>
       <c r="B58" s="6">
         <v>44340</v>
       </c>
@@ -1713,7 +1729,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="35"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="6">
         <v>44343</v>
       </c>
@@ -1728,7 +1744,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="34">
+      <c r="A60" s="36">
         <v>22</v>
       </c>
       <c r="B60" s="21" t="s">
@@ -1745,7 +1761,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="36"/>
+      <c r="A61" s="37"/>
       <c r="B61" s="3" t="s">
         <v>1</v>
       </c>
@@ -1758,7 +1774,7 @@
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="6">
         <v>44347</v>
       </c>
@@ -1773,7 +1789,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="35"/>
+      <c r="A63" s="38"/>
       <c r="B63" s="6">
         <v>44350</v>
       </c>
@@ -1788,7 +1804,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="34">
+      <c r="A64" s="36">
         <v>23</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -1803,7 +1819,7 @@
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="35"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="14">
         <v>44358</v>
       </c>
@@ -1818,7 +1834,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B66" s="31">
@@ -1835,7 +1851,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="35"/>
+      <c r="A67" s="38"/>
       <c r="B67" s="31">
         <v>44383</v>
       </c>
@@ -1851,11 +1867,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A27:A30"/>
@@ -1869,6 +1880,11 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update api_inv.md; add security design principles
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Dropbox\_Schule\_zhaw\21FS\BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46EB088-D7E1-4724-B873-685F4DA13E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8176BC5F-BF16-40C7-B69C-26FE8B670A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3250" windowWidth="26570" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
+    <workbookView xWindow="2920" yWindow="2860" windowWidth="26570" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,29 +440,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BAD31A-C75F-4250-BB4F-3B614CCB7A8D}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:D53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,11 +803,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -879,7 +879,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="36">
+      <c r="A5" s="37">
         <v>8</v>
       </c>
       <c r="B5" s="3">
@@ -896,7 +896,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="6">
         <v>44249</v>
       </c>
@@ -926,7 +926,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="36">
+      <c r="A8" s="37">
         <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -943,7 +943,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="37"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="6">
         <v>44256</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="36">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
@@ -993,7 +993,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="37"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="9" t="s">
         <v>1</v>
       </c>
@@ -1011,7 +1011,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="6">
         <v>44263</v>
       </c>
@@ -1047,7 +1047,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="35">
+      <c r="A15" s="41">
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -1064,7 +1064,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
@@ -1079,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="6">
         <v>44270</v>
       </c>
@@ -1094,7 +1094,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="6">
         <v>44273</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="36">
+      <c r="A19" s="37">
         <v>12</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -1126,7 +1126,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="37"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="9" t="s">
         <v>1</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="37"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="6">
         <v>44277</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="36">
+      <c r="A23" s="37">
         <v>13</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="9" t="s">
         <v>1</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="37"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="6">
         <v>44284</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="36">
+      <c r="A27" s="37">
         <v>14</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -1250,7 +1250,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="37"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="37"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="6">
         <v>44291</v>
       </c>
@@ -1295,7 +1295,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="36">
+      <c r="A31" s="37">
         <v>15</v>
       </c>
       <c r="B31" s="21" t="s">
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="37"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="9" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="37"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="6">
         <v>44298</v>
       </c>
@@ -1357,7 +1357,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="36">
+      <c r="A35" s="37">
         <v>16</v>
       </c>
       <c r="B35" s="21" t="s">
@@ -1374,7 +1374,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="37"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="9" t="s">
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="37"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="6">
         <v>44305</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="36">
+      <c r="A39" s="37">
         <v>17</v>
       </c>
       <c r="B39" s="21" t="s">
@@ -1436,7 +1436,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="37"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
@@ -1451,17 +1451,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="37"/>
-      <c r="B41" s="39">
+      <c r="A41" s="39"/>
+      <c r="B41" s="34">
         <v>44312</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="41" t="s">
+      <c r="D41" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="36">
+      <c r="A43" s="37">
         <v>18</v>
       </c>
       <c r="B43" s="21" t="s">
@@ -1498,7 +1498,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="37"/>
+      <c r="A44" s="39"/>
       <c r="B44" s="9" t="s">
         <v>1</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="37"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="6">
         <v>44319</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="36">
+      <c r="A47" s="37">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="37"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="37"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="6">
         <v>44326</v>
       </c>
@@ -1591,21 +1591,21 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="38"/>
-      <c r="B50" s="39">
+      <c r="B50" s="34">
         <v>44329</v>
       </c>
-      <c r="C50" s="40" t="s">
+      <c r="C50" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D50" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="41" t="s">
+      <c r="D50" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="36" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="36">
+      <c r="A51" s="37">
         <v>20</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -1622,7 +1622,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="37"/>
+      <c r="A52" s="39"/>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="37"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="37"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="6">
         <v>44333</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="36">
+      <c r="A56" s="37">
         <v>21</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="37"/>
+      <c r="A57" s="39"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -1714,17 +1714,17 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="37"/>
-      <c r="B58" s="6">
+      <c r="A58" s="39"/>
+      <c r="B58" s="34">
         <v>44340</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="8" t="s">
+      <c r="D58" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1744,7 +1744,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="36">
+      <c r="A60" s="37">
         <v>22</v>
       </c>
       <c r="B60" s="21" t="s">
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="37"/>
+      <c r="A61" s="39"/>
       <c r="B61" s="3" t="s">
         <v>1</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="37"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="6">
         <v>44347</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="36">
+      <c r="A64" s="37">
         <v>23</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B66" s="31">
@@ -1867,6 +1867,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A5:A7"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A27:A30"/>
@@ -1880,11 +1885,6 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A51:A55"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename meeting, correct time table
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Dropbox\_Schule\_zhaw\21FS\BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8176BC5F-BF16-40C7-B69C-26FE8B670A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D66C5B9-90DA-482E-A243-4D6A098A975D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2860" windowWidth="26570" windowHeight="16510" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
+    <workbookView xWindow="-23800" yWindow="5530" windowWidth="28800" windowHeight="15460" xr2:uid="{2AF3C5B4-B315-43CA-B613-02DEF33EAFB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="48">
   <si>
     <t>Kickoff Meeting</t>
   </si>
@@ -41,18 +41,12 @@
     <t>-</t>
   </si>
   <si>
-    <t>Preparation Kickoff Meeting</t>
-  </si>
-  <si>
     <t>Meetings</t>
   </si>
   <si>
     <t>Reserve</t>
   </si>
   <si>
-    <t>Research</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>S,D,N</t>
   </si>
   <si>
-    <t>Coding</t>
-  </si>
-  <si>
     <t>Organisational Meeting</t>
   </si>
   <si>
@@ -86,21 +77,9 @@
     <t>Abgabe BA - 17:00 Uhr</t>
   </si>
   <si>
-    <t>26, 27</t>
-  </si>
-  <si>
     <t>wöchentliches Meeting</t>
   </si>
   <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>Informationen sammeln zu DIVA.EXCHANGE, irohad, I2P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA anfangen zu schreiben, Inhaltsverzeichnis und Struktur </t>
-  </si>
-  <si>
     <t>Ausgangslage und Ziel</t>
   </si>
   <si>
@@ -170,12 +149,6 @@
     <t>Do</t>
   </si>
   <si>
-    <t>Präsentation Zeitfenster Start</t>
-  </si>
-  <si>
-    <t>Präsentation Zeitfenster Ende</t>
-  </si>
-  <si>
     <t>S,B</t>
   </si>
   <si>
@@ -183,13 +156,34 @@
   </si>
   <si>
     <t>DFD und Threat-Modelling</t>
+  </si>
+  <si>
+    <t>Präsentation &amp; Verteidigung BA</t>
+  </si>
+  <si>
+    <t>BA anfangen zu schreiben, Inhaltsverzeichnis und Struktur</t>
+  </si>
+  <si>
+    <t>Informationen sammeln zu DIVA.EXCHANGE, Iroha, I2P</t>
+  </si>
+  <si>
+    <t>Vorbereitung Kickoff Meeting</t>
+  </si>
+  <si>
+    <t>Arbeit</t>
+  </si>
+  <si>
+    <t>Forschung</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,13 +216,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -275,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -298,48 +285,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -422,9 +372,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -440,22 +387,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -784,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BAD31A-C75F-4250-BB4F-3B614CCB7A8D}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,7 +727,7 @@
     <col min="1" max="1" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.08984375" style="1" customWidth="1"/>
     <col min="5" max="6" width="9.1796875" style="1"/>
     <col min="7" max="7" width="11.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="35" style="1" customWidth="1"/>
@@ -803,130 +735,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="29">
+        <v>50</v>
+      </c>
+      <c r="B3" s="28">
+        <v>44181</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="29">
+        <v>6</v>
+      </c>
+      <c r="B4" s="28">
+        <v>44236</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="28">
-        <v>50</v>
-      </c>
-      <c r="B3" s="29">
-        <v>44181</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="28">
-        <v>6</v>
-      </c>
-      <c r="B4" s="29">
-        <v>44236</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="37">
+      <c r="A5" s="35">
         <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>44249</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="6">
         <v>44249</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="6">
         <v>44252</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="37">
+      <c r="A8" s="35">
         <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -936,118 +868,118 @@
         <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="39"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="6">
         <v>44256</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="6">
         <v>44259</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="35">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="35"/>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="37">
-        <v>10</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
-      <c r="B12" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="6">
         <v>44263</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="6">
         <v>44266</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="41">
+      <c r="A15" s="35">
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
@@ -1057,14 +989,14 @@
         <v>1</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
@@ -1072,61 +1004,61 @@
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="41"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="6">
         <v>44270</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="41"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="6">
         <v>44273</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="35">
+        <v>12</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="37">
-        <v>12</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>25</v>
-      </c>
       <c r="E19" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="39"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="9" t="s">
         <v>1</v>
       </c>
@@ -1134,44 +1066,44 @@
         <v>1</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="39"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="6">
         <v>44277</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="6">
         <v>44280</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="37">
+      <c r="A23" s="35">
         <v>13</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -1181,14 +1113,14 @@
         <v>1</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="39"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="9" t="s">
         <v>1</v>
       </c>
@@ -1196,44 +1128,44 @@
         <v>1</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="39"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="6">
         <v>44284</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="38"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="6">
         <v>44287</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="37">
+      <c r="A27" s="35">
         <v>14</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -1243,14 +1175,14 @@
         <v>1</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="39"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
@@ -1258,44 +1190,44 @@
         <v>1</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="39"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="6">
         <v>44291</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="6">
         <v>44294</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="37">
+      <c r="A31" s="35">
         <v>15</v>
       </c>
       <c r="B31" s="21" t="s">
@@ -1305,14 +1237,14 @@
         <v>1</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="39"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="9" t="s">
         <v>1</v>
       </c>
@@ -1320,44 +1252,44 @@
         <v>1</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="6">
         <v>44298</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="38"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="6">
         <v>44301</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="37">
+      <c r="A35" s="35">
         <v>16</v>
       </c>
       <c r="B35" s="21" t="s">
@@ -1367,14 +1299,14 @@
         <v>1</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="39"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="9" t="s">
         <v>1</v>
       </c>
@@ -1382,44 +1314,44 @@
         <v>1</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="39"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="6">
         <v>44305</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="38"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="6">
         <v>44308</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="37">
+      <c r="A39" s="35">
         <v>17</v>
       </c>
       <c r="B39" s="21" t="s">
@@ -1429,14 +1361,14 @@
         <v>1</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="39"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
@@ -1444,46 +1376,46 @@
         <v>1</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="39"/>
-      <c r="B41" s="34">
+      <c r="A41" s="35"/>
+      <c r="B41" s="6">
         <v>44312</v>
       </c>
-      <c r="C41" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="36" t="s">
-        <v>10</v>
+      <c r="C41" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="6">
         <v>44315</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="35">
         <v>18</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="37">
-        <v>18</v>
-      </c>
       <c r="B43" s="21" t="s">
         <v>1</v>
       </c>
@@ -1491,14 +1423,14 @@
         <v>1</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="39"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="9" t="s">
         <v>1</v>
       </c>
@@ -1506,44 +1438,44 @@
         <v>1</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="39"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="6">
         <v>44319</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="38"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="6">
         <v>44322</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="37">
+      <c r="A47" s="35">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
@@ -1553,14 +1485,14 @@
         <v>1</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="39"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
@@ -1568,44 +1500,44 @@
         <v>1</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="39"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="6">
         <v>44326</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="38"/>
-      <c r="B50" s="34">
+      <c r="A50" s="35"/>
+      <c r="B50" s="6">
         <v>44329</v>
       </c>
-      <c r="C50" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="36" t="s">
-        <v>42</v>
+      <c r="C50" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="37">
+      <c r="A51" s="35">
         <v>20</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -1615,14 +1547,14 @@
         <v>1</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="39"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
@@ -1630,14 +1562,14 @@
         <v>1</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="39"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="35"/>
       <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
@@ -1645,44 +1577,44 @@
         <v>1</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="39"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="6">
         <v>44333</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="38"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="6">
         <v>44336</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="37">
+      <c r="A56" s="35">
         <v>21</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -1692,14 +1624,14 @@
         <v>1</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="39"/>
+      <c r="A57" s="35"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -1707,44 +1639,44 @@
         <v>1</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="39"/>
-      <c r="B58" s="34">
+      <c r="A58" s="35"/>
+      <c r="B58" s="6">
         <v>44340</v>
       </c>
-      <c r="C58" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="36" t="s">
-        <v>10</v>
+      <c r="C58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="38"/>
+      <c r="A59" s="35"/>
       <c r="B59" s="6">
         <v>44343</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="37">
+      <c r="A60" s="35">
         <v>22</v>
       </c>
       <c r="B60" s="21" t="s">
@@ -1754,14 +1686,14 @@
         <v>1</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="39"/>
+      <c r="A61" s="35"/>
       <c r="B61" s="3" t="s">
         <v>1</v>
       </c>
@@ -1769,42 +1701,42 @@
         <v>1</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="39"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="6">
         <v>44347</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="38"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="6">
         <v>44350</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="37">
+      <c r="A64" s="35">
         <v>23</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -1814,65 +1746,44 @@
         <v>1</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="38"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="14">
         <v>44358</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" s="31">
-        <v>44378</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E66" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="38"/>
-      <c r="B67" s="31">
-        <v>44383</v>
-      </c>
-      <c r="C67" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="33">
+        <v>26</v>
+      </c>
+      <c r="B66" s="30">
+        <v>44379</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A66:A67"/>
+  <mergeCells count="17">
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A23:A26"/>
@@ -1885,6 +1796,11 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>